<commit_message>
Add spreadsheet with planning and timing
</commit_message>
<xml_diff>
--- a/WPF Workshop.xlsx
+++ b/WPF Workshop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_mts\repos\wpf-workshop-solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E52577C-9403-4793-87E4-C803AB4AEF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEB1566-1531-48B7-9C3B-40266C32A2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3770" yWindow="2630" windowWidth="25990" windowHeight="16900" xr2:uid="{5EA1D85C-AEE8-44BD-88F2-BFE6E1EF4739}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="B2:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Working on Unit 3
</commit_message>
<xml_diff>
--- a/WPF Workshop.xlsx
+++ b/WPF Workshop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_mts\repos\wpf-workshop-solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEB1566-1531-48B7-9C3B-40266C32A2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C5CCDC-2BCC-40E3-AD95-16F6DEE863EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3770" yWindow="2630" windowWidth="25990" windowHeight="16900" xr2:uid="{5EA1D85C-AEE8-44BD-88F2-BFE6E1EF4739}"/>
+    <workbookView xWindow="42170" yWindow="2630" windowWidth="25990" windowHeight="16900" xr2:uid="{5EA1D85C-AEE8-44BD-88F2-BFE6E1EF4739}"/>
   </bookViews>
   <sheets>
     <sheet name="Timing" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Unit</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>Actual</t>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -201,26 +204,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B537126-BC96-477F-A5DE-464A92496261}">
-  <dimension ref="B2:L29"/>
+  <dimension ref="B2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -548,27 +549,30 @@
     <col min="8" max="8" width="11.05078125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="E2" s="1" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="J2" s="2" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="J2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="2" t="s">
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="10"/>
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F3" t="s">
@@ -577,23 +581,26 @@
       <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B4">
         <v>1</v>
       </c>
@@ -603,7 +610,7 @@
       <c r="D4">
         <v>9</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <f>D4*3</f>
         <v>27</v>
       </c>
@@ -613,41 +620,45 @@
       <c r="G4">
         <v>10</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="2">
         <f>SUM(E4:G4)</f>
         <v>62</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="9">
         <v>0.3520833333333333</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="4">
         <v>0.36944444444444446</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="3">
         <v>0.37638888888888888</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="8" t="s">
+      <c r="N4">
+        <f>4+4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="H5" s="4">
-        <v>10</v>
-      </c>
-      <c r="I5" s="6">
+      <c r="E5" s="2"/>
+      <c r="H5" s="2">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3">
         <v>0.37638888888888888</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="6">
+      <c r="J5" s="9"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="3">
         <v>0.3833333333333333</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B6">
         <v>2</v>
       </c>
@@ -657,7 +668,7 @@
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <f>D6*3</f>
         <v>15</v>
       </c>
@@ -667,41 +678,44 @@
       <c r="G6">
         <v>10</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="2">
         <f>SUM(E6:G6)</f>
         <v>45</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="3">
         <v>0.3833333333333333</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="9">
         <v>0.39374999999999999</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="4">
         <v>0.40763888888888888</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="3">
         <v>0.4145833333333333</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" s="8" t="s">
+      <c r="N6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="H7" s="4">
-        <v>10</v>
-      </c>
-      <c r="I7" s="6">
+      <c r="E7" s="2"/>
+      <c r="H7" s="2">
+        <v>10</v>
+      </c>
+      <c r="I7" s="3">
         <v>0.4145833333333333</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="6">
+      <c r="J7" s="9"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="3">
         <v>0.42152777777777778</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
         <v>3</v>
       </c>
@@ -711,7 +725,7 @@
       <c r="D8">
         <v>6</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <f>D8*3</f>
         <v>18</v>
       </c>
@@ -721,41 +735,44 @@
       <c r="G8">
         <v>10</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="2">
         <f>SUM(E8:G8)</f>
         <v>48</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="4">
         <v>0.42152777777777778</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="9">
         <v>0.43402777777777773</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="4">
         <v>0.44791666666666669</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="3">
         <v>0.4548611111111111</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C9" s="8" t="s">
+      <c r="N8" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="H9" s="4">
-        <v>10</v>
-      </c>
-      <c r="I9" s="7">
+      <c r="E9" s="2"/>
+      <c r="H9" s="2">
+        <v>10</v>
+      </c>
+      <c r="I9" s="4">
         <v>0.4548611111111111</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="6">
+      <c r="J9" s="9"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="3">
         <v>0.46180555555555558</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
         <v>4</v>
       </c>
@@ -765,7 +782,7 @@
       <c r="D10">
         <v>5</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <f>D10*3</f>
         <v>15</v>
       </c>
@@ -775,44 +792,44 @@
       <c r="G10">
         <v>10</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="2">
         <f>SUM(E10:G10)</f>
         <v>40</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="3">
         <v>0.46180555555555558</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="9">
         <v>0.47222222222222227</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="4">
         <v>0.4826388888888889</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="3">
         <v>0.48958333333333331</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C11" s="9" t="s">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11">
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8">
         <v>60</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="3">
         <v>0.48958333333333331</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="6">
+      <c r="J11" s="9"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="3">
         <v>0.53125</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B12">
         <v>5</v>
       </c>
@@ -822,7 +839,7 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <f>D12*3</f>
         <v>9</v>
       </c>
@@ -832,41 +849,41 @@
       <c r="G12">
         <v>10</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="2">
         <f>SUM(E12:G12)</f>
         <v>34</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="3">
         <v>0.53125</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="9">
         <v>0.53749999999999998</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="4">
         <v>0.54791666666666672</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="3">
         <v>0.55486111111111114</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C13" s="8" t="s">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="H13" s="4">
-        <v>10</v>
-      </c>
-      <c r="I13" s="6">
+      <c r="E13" s="2"/>
+      <c r="H13" s="2">
+        <v>10</v>
+      </c>
+      <c r="I13" s="3">
         <v>0.55486111111111114</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="6">
+      <c r="J13" s="9"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="3">
         <v>0.56180555555555556</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B14">
         <v>6</v>
       </c>
@@ -876,7 +893,7 @@
       <c r="D14">
         <v>3</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="2">
         <f>D14*3</f>
         <v>9</v>
       </c>
@@ -886,41 +903,41 @@
       <c r="G14">
         <v>10</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="2">
         <f>SUM(E14:G14)</f>
         <v>34</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="3">
         <v>0.56180555555555556</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="9">
         <v>0.56805555555555554</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="4">
         <v>0.57847222222222217</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="3">
         <v>0.5854166666666667</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C15" s="8" t="s">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="H15" s="4">
-        <v>10</v>
-      </c>
-      <c r="I15" s="6">
+      <c r="E15" s="2"/>
+      <c r="H15" s="2">
+        <v>10</v>
+      </c>
+      <c r="I15" s="3">
         <v>0.5854166666666667</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="6">
+      <c r="J15" s="9"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="3">
         <v>0.59236111111111112</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B16">
         <v>7</v>
       </c>
@@ -930,7 +947,7 @@
       <c r="D16">
         <v>5</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="2">
         <f>D16*3</f>
         <v>15</v>
       </c>
@@ -940,37 +957,37 @@
       <c r="G16">
         <v>10</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="2">
         <f>SUM(E16:G16)</f>
         <v>40</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="3">
         <v>0.59236111111111112</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="9">
         <v>0.60277777777777775</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="4">
         <v>0.61319444444444449</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="3">
         <v>0.62013888888888891</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="H17" s="4">
-        <v>10</v>
-      </c>
-      <c r="I17" s="6">
+      <c r="E17" s="2"/>
+      <c r="H17" s="2">
+        <v>10</v>
+      </c>
+      <c r="I17" s="3">
         <v>0.62013888888888891</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="6">
+      <c r="J17" s="9"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="3">
         <v>0.62708333333333333</v>
       </c>
     </row>
@@ -984,7 +1001,7 @@
       <c r="D18">
         <v>5</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <f>D18*3</f>
         <v>15</v>
       </c>
@@ -994,37 +1011,37 @@
       <c r="G18">
         <v>10</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="2">
         <f>SUM(E18:G18)</f>
         <v>45</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="3">
         <v>0.62708333333333333</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="9">
         <v>0.63750000000000007</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="4">
         <v>0.65138888888888891</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="3">
         <v>0.65833333333333333</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="H19" s="4">
-        <v>10</v>
-      </c>
-      <c r="I19" s="6">
+      <c r="E19" s="2"/>
+      <c r="H19" s="2">
+        <v>10</v>
+      </c>
+      <c r="I19" s="3">
         <v>0.65833333333333333</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="6">
+      <c r="J19" s="9"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="3">
         <v>0.66527777777777775</v>
       </c>
     </row>
@@ -1038,7 +1055,7 @@
       <c r="D20">
         <v>4</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2">
         <f>D20*3</f>
         <v>12</v>
       </c>
@@ -1048,20 +1065,20 @@
       <c r="G20">
         <v>10</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="2">
         <f>SUM(E20:G20)</f>
         <v>37</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="3">
         <v>0.66527777777777775</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="9">
         <v>0.67361111111111116</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="4">
         <v>0.68402777777777779</v>
       </c>
-      <c r="L20" s="6">
+      <c r="L20" s="3">
         <v>0.69097222222222221</v>
       </c>
     </row>
@@ -1069,13 +1086,13 @@
       <c r="B21">
         <v>10</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" t="s">
         <v>28</v>
       </c>
       <c r="D21">
         <v>3</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <f>D21*3</f>
         <v>9</v>
       </c>
@@ -1085,18 +1102,18 @@
       <c r="G21">
         <v>10</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="2">
         <f>SUM(E21:G21)</f>
         <v>19</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="3">
         <v>0.69097222222222221</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="9">
         <v>0.6972222222222223</v>
       </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="6">
+      <c r="K21" s="4"/>
+      <c r="L21" s="3">
         <v>0.70416666666666661</v>
       </c>
     </row>
@@ -1121,7 +1138,7 @@
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add unit 6 content
</commit_message>
<xml_diff>
--- a/WPF Workshop.xlsx
+++ b/WPF Workshop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_mts\repos\wpf-workshop-solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C5CCDC-2BCC-40E3-AD95-16F6DEE863EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6108420-8DBB-4DE1-966F-D8A3C45A7ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42170" yWindow="2630" windowWidth="25990" windowHeight="16900" xr2:uid="{5EA1D85C-AEE8-44BD-88F2-BFE6E1EF4739}"/>
   </bookViews>
@@ -204,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -221,7 +221,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +538,7 @@
   <dimension ref="B2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -751,7 +750,7 @@
       <c r="L8" s="3">
         <v>0.4548611111111111</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8">
         <v>7</v>
       </c>
     </row>
@@ -807,6 +806,9 @@
       </c>
       <c r="L10" s="3">
         <v>0.48958333333333331</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -864,6 +866,9 @@
       </c>
       <c r="L12" s="3">
         <v>0.55486111111111114</v>
+      </c>
+      <c r="N12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">

</xml_diff>